<commit_message>
Tweak some values as a result of testing
</commit_message>
<xml_diff>
--- a/misc/LevellingCurves.xlsx
+++ b/misc/LevellingCurves.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louis Thie\workspace\SWEN224\RoomScape\misc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
@@ -15,9 +10,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -81,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,21 +126,11 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-NZ"/>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -174,12 +159,10 @@
         </a:p>
       </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -824,35 +807,25 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-77F1-4892-870A-2398192240AA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="371007248"/>
-        <c:axId val="371003968"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="101595008"/>
+        <c:axId val="101596544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="371007248"/>
+        <c:axId val="101595008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -887,19 +860,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371003968"/>
+        <c:crossAx val="101596544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="371003968"/>
+        <c:axId val="101596544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -917,7 +888,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -946,7 +916,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371007248"/>
+        <c:crossAx val="101595008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -960,7 +930,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -989,28 +958,18 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-NZ"/>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1039,12 +998,10 @@
         </a:p>
       </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1689,35 +1646,25 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3424-4063-ACE7-4E2604062D6B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="367935632"/>
-        <c:axId val="367927432"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="101621120"/>
+        <c:axId val="144778368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="367935632"/>
+        <c:axId val="101621120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1752,19 +1699,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="367927432"/>
+        <c:crossAx val="144778368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="367927432"/>
+        <c:axId val="144778368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1782,7 +1727,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1811,7 +1755,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="367935632"/>
+        <c:crossAx val="101621120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1825,7 +1769,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1854,28 +1797,18 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-NZ"/>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1904,12 +1837,10 @@
         </a:p>
       </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2554,35 +2485,25 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-922F-4792-A180-AD9CDA08BF87}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="479235032"/>
-        <c:axId val="479236344"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="144807040"/>
+        <c:axId val="144808576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="479235032"/>
+        <c:axId val="144807040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2617,19 +2538,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479236344"/>
+        <c:crossAx val="144808576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="479236344"/>
+        <c:axId val="144808576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2647,7 +2566,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2676,7 +2594,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479235032"/>
+        <c:crossAx val="144807040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2690,7 +2608,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2719,7 +2636,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4531,7 +4448,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -4583,7 +4500,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -4777,27 +4694,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="15" max="15" width="12.42578125" customWidth="1"/>
     <col min="16" max="16" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4829,7 +4746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4864,7 +4781,7 @@
         <v>1.974</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4881,7 +4798,7 @@
         <v>10.465018489910968</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4898,7 +4815,7 @@
         <v>10.951661199417837</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4915,7 +4832,7 @@
         <v>11.460933694714821</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4932,7 +4849,7 @@
         <v>11.993888302683416</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4949,7 +4866,7 @@
         <v>12.551626285350881</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4966,7 +4883,7 @@
         <v>13.135300115464952</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4983,7 +4900,7 @@
         <v>13.74611585788703</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5000,7 +4917,7 @@
         <v>14.385335661724612</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5017,7 +4934,7 @@
         <v>15.054280368352359</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5034,7 +4951,7 @@
         <v>15.754332240711118</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5051,7 +4968,7 @@
         <v>16.486937819524233</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5068,7 +4985,7 @@
         <v>17.25361091233334</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5085,7 +5002,7 @@
         <v>18.055935721529799</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5102,7 +5019,7 @@
         <v>18.895570117845324</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5119,7 +5036,7 @@
         <v>19.774249066066044</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5136,7 +5053,7 @@
         <v>20.693788210048581</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5153,7 +5070,7 @@
         <v>21.656087624445988</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5170,7 +5087,7 @@
         <v>22.663135740895932</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5187,7 +5104,7 @@
         <v>23.717013456783796</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5204,7 +5121,7 @@
         <v>24.819898435070964</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5221,7 +5138,7 @@
         <v>25.974069604072977</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5238,7 +5155,7 @@
         <v>27.181911866485823</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5255,7 +5172,7 @@
         <v>28.445921027390444</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5272,7 +5189,7 @@
         <v>29.768708951418798</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5289,7 +5206,7 @@
         <v>31.153008959737594</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5306,7 +5223,7 @@
         <v>32.601681478001595</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5323,7 +5240,7 @@
         <v>34.117719946947439</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5340,7 +5257,7 @@
         <v>35.704257007840916</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5357,7 +5274,7 @@
         <v>37.36457097555882</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5374,7 +5291,7 @@
         <v>39.102092612681382</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5391,7 +5308,7 @@
         <v>40.920412218592162</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5408,7 +5325,7 @@
         <v>42.82328704823454</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5425,7 +5342,7 @@
         <v>44.814649075853907</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5442,7 +5359,7 @@
         <v>46.898613119768271</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5459,7 +5376,7 @@
         <v>49.0794853449556</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5476,7 +5393,7 @@
         <v>51.361772161027439</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5493,7 +5410,7 @@
         <v>53.75018953397467</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5510,7 +5427,7 @@
         <v>56.249672730926356</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5527,7 +5444,7 @@
         <v>58.865386518058529</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5544,7 +5461,7 @@
         <v>61.602735832723788</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5561,7 +5478,7 @@
         <v>64.467376951855499</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5578,7 +5495,7 @@
         <v>67.465229179722755</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5595,7 +5512,7 @@
         <v>70.602487079187981</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5612,7 +5529,7 @@
         <v>73.885633271740261</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5629,7 +5546,7 @@
         <v>77.321451832754235</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5646,7 +5563,7 @@
         <v>80.917042309653354</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5663,7 +5580,7 @@
         <v>84.67983439194299</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5680,7 +5597,7 @@
         <v>88.617603263428151</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5697,7 +5614,7 @@
         <v>92.738485668337034</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5714,7 +5631,7 @@
         <v>97.050996724549066</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5731,7 +5648,7 @@
         <v>101.56404751866933</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5748,7 +5665,7 @@
         <v>106.28696351930719</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5765,7 +5682,7 @@
         <v>111.22950384660406</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5782,7 +5699,7 @@
         <v>116.40188143783348</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>56</v>
       </c>
@@ -5799,7 +5716,7 @@
         <v>121.81478415073521</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5816,7 +5733,7 @@
         <v>127.47939684819566</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5833,7 +5750,7 @@
         <v>133.40742450990646</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5850,7 +5767,7 @@
         <v>139.61111641875721</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5867,7 +5784,7 @@
         <v>146.10329147194074</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5884,7 +5801,7 @@
         <v>152.89736466907115</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5901,7 +5818,7 @@
         <v>160.00737483204873</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64">
         <v>63</v>
       </c>
@@ -5918,7 +5835,7 @@
         <v>167.44801361395065</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65">
         <v>64</v>
       </c>
@@ -5935,7 +5852,7 @@
         <v>175.23465585688561</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66">
         <v>65</v>
       </c>
@@ -5952,7 +5869,7 @@
         <v>183.3833913615492</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67">
         <v>66</v>
       </c>
@@ -5969,7 +5886,7 @@
         <v>191.9110581341192</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68">
         <v>67</v>
       </c>
@@ -5986,7 +5903,7 @@
         <v>200.8352771791933</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69">
         <v>68</v>
       </c>
@@ -6003,7 +5920,7 @@
         <v>210.17448891066547</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70">
         <v>69</v>
       </c>
@@ -6020,7 +5937,7 @@
         <v>219.94799125577003</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71">
         <v>70</v>
       </c>
@@ -6037,7 +5954,7 @@
         <v>230.17597953104058</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6054,7 +5971,7 @@
         <v>240.87958817257109</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6071,7 +5988,7 @@
         <v>252.08093440680943</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74">
         <v>73</v>
       </c>
@@ -6088,7 +6005,7 @@
         <v>263.8031639521293</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75">
         <v>74</v>
       </c>
@@ -6105,7 +6022,7 @@
         <v>276.07049884560485</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76">
         <v>75</v>
       </c>
@@ -6122,7 +6039,7 @@
         <v>288.90828749381996</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77">
         <v>76</v>
       </c>
@@ -6139,7 +6056,7 @@
         <v>302.34305705113377</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78">
         <v>77</v>
       </c>
@@ -6156,7 +6073,7 @@
         <v>316.402568233632</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79">
         <v>78</v>
       </c>
@@ -6173,7 +6090,7 @@
         <v>331.11587268202788</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80">
         <v>79</v>
       </c>
@@ -6190,7 +6107,7 @@
         <v>346.51337299204226</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81">
         <v>80</v>
       </c>
@@ -6207,7 +6124,7 @@
         <v>362.62688553631392</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82">
         <v>81</v>
       </c>
@@ -6224,7 +6141,7 @@
         <v>379.48970620763509</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4">
       <c r="A83">
         <v>82</v>
       </c>
@@ -6241,7 +6158,7 @@
         <v>397.13667921937798</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84">
         <v>83</v>
       </c>
@@ -6258,7 +6175,7 @@
         <v>415.60426910526326</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85">
         <v>84</v>
       </c>
@@ -6275,7 +6192,7 @@
         <v>434.9306360672511</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86">
         <v>85</v>
       </c>
@@ -6292,7 +6209,7 @@
         <v>455.15571482725176</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87">
         <v>86</v>
       </c>
@@ -6309,7 +6226,7 @@
         <v>476.32129714558391</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88">
         <v>87</v>
       </c>
@@ -6326,7 +6243,7 @@
         <v>498.47111817669042</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89">
         <v>88</v>
       </c>
@@ -6343,7 +6260,7 @@
         <v>521.65094684056623</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90">
         <v>89</v>
       </c>
@@ -6360,7 +6277,7 @@
         <v>545.90868039660847</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91">
         <v>90</v>
       </c>
@@ -6377,7 +6294,7 @@
         <v>571.29444341534065</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92">
         <v>91</v>
       </c>
@@ -6394,7 +6311,7 @@
         <v>597.86069135249375</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93">
         <v>92</v>
       </c>
@@ -6411,7 +6328,7 @@
         <v>625.66231893947918</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94">
         <v>93</v>
       </c>
@@ -6428,7 +6345,7 @@
         <v>654.75677361422299</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95">
         <v>94</v>
       </c>
@@ -6445,7 +6362,7 @@
         <v>685.20417422672892</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96">
         <v>95</v>
       </c>
@@ -6462,7 +6379,7 @@
         <v>717.06743526468836</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97">
         <v>96</v>
       </c>
@@ -6479,7 +6396,7 @@
         <v>750.41239685580081</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98">
         <v>97</v>
       </c>
@@ -6496,7 +6413,7 @@
         <v>785.30796081543508</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99">
         <v>98</v>
       </c>
@@ -6513,7 +6430,7 @@
         <v>821.82623302078082</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100">
         <v>99</v>
       </c>
@@ -6530,7 +6447,7 @@
         <v>860.04267240563524</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101">
         <v>100</v>
       </c>
@@ -6554,14 +6471,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
@@ -6576,7 +6493,7 @@
     <col min="18" max="18" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -6626,7 +6543,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -6643,10 +6560,10 @@
         <v>45</v>
       </c>
       <c r="R2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>1</v>
       </c>
@@ -6691,7 +6608,7 @@
         <v>166.49999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>2</v>
       </c>
@@ -6736,7 +6653,7 @@
         <v>174.34690325047478</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>3</v>
       </c>
@@ -6781,7 +6698,7 @@
         <v>182.56361965784046</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>4</v>
       </c>
@@ -6826,7 +6743,7 @@
         <v>191.16757797923108</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>5</v>
       </c>
@@ -6871,7 +6788,7 @@
         <v>200.17702836379934</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>6</v>
       </c>
@@ -6916,7 +6833,7 @@
         <v>209.6110810637289</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>7</v>
       </c>
@@ -6961,7 +6878,7 @@
         <v>219.48974696964197</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>8</v>
       </c>
@@ -7006,7 +6923,7 @@
         <v>229.83398005638051</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>9</v>
       </c>
@@ -7051,7 +6968,7 @@
         <v>240.66572182919705</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>10</v>
       </c>
@@ -7096,7 +7013,7 @@
         <v>252.00794786462879</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>11</v>
       </c>
@@ -7141,7 +7058,7 @@
         <v>263.8847165447757</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>12</v>
       </c>
@@ -7186,7 +7103,7 @@
         <v>276.3212200883541</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>13</v>
       </c>
@@ -7231,7 +7148,7 @@
         <v>289.34383798677118</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>14</v>
       </c>
@@ -7276,7 +7193,7 @@
         <v>302.98019295856216</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>15</v>
       </c>
@@ -7321,7 +7238,7 @@
         <v>317.25920954088105</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>16</v>
       </c>
@@ -7366,7 +7283,7 @@
         <v>332.21117544231851</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>17</v>
       </c>
@@ -7411,7 +7328,7 @@
         <v>347.86780578719754</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>18</v>
       </c>
@@ -7456,7 +7373,7 @@
         <v>364.26231038760045</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>19</v>
       </c>
@@ -7501,7 +7418,7 @@
         <v>381.42946418583438</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>20</v>
       </c>
@@ -7546,7 +7463,7 @@
         <v>399.40568101674523</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>21</v>
       </c>
@@ -7591,7 +7508,7 @@
         <v>418.22909084634512</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>22</v>
       </c>
@@ -7636,7 +7553,7 @@
         <v>437.93962065058099</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>23</v>
       </c>
@@ -7681,7 +7598,7 @@
         <v>458.57907910580496</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>24</v>
       </c>
@@ -7726,7 +7643,7 @@
         <v>480.19124527058005</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>25</v>
       </c>
@@ -7771,7 +7688,7 @@
         <v>502.82196144693575</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>26</v>
       </c>
@@ -7816,7 +7733,7 @@
         <v>526.51923041803559</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>27</v>
       </c>
@@ -7861,7 +7778,7 @@
         <v>551.33331726851452</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>28</v>
       </c>
@@ -7906,7 +7823,7 @@
         <v>577.31685600346543</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31">
         <v>29</v>
       </c>
@@ -7951,7 +7868,7 @@
         <v>604.52496119221894</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32">
         <v>30</v>
       </c>
@@ -7996,7 +7913,7 @@
         <v>633.01534487373499</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33">
         <v>31</v>
       </c>
@@ -8041,7 +7958,7 @@
         <v>662.8484389715735</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34">
         <v>32</v>
       </c>
@@ -8086,7 +8003,7 @@
         <v>694.08752347810889</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35">
         <v>33</v>
       </c>
@@ -8131,7 +8048,7 @@
         <v>726.79886067987673</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36">
         <v>34</v>
       </c>
@@ -8176,7 +8093,7 @@
         <v>761.05183570876784</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37">
         <v>35</v>
       </c>
@@ -8221,7 +8138,7 @@
         <v>796.91910371719359</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38">
         <v>36</v>
       </c>
@@ -8266,7 +8183,7 @@
         <v>834.47674398940899</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39">
         <v>37</v>
       </c>
@@ -8311,7 +8228,7 @@
         <v>873.80442131587108</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40">
         <v>38</v>
       </c>
@@ -8356,7 +8273,7 @@
         <v>914.98555497294615</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41">
         <v>39</v>
       </c>
@@ -8401,7 +8318,7 @@
         <v>958.10749566636639</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42">
         <v>40</v>
       </c>
@@ -8446,7 +8363,7 @@
         <v>1003.2617108138065</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43">
         <v>41</v>
       </c>
@@ -8491,7 +8408,7 @@
         <v>1050.5439785595215</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="A44">
         <v>42</v>
       </c>
@@ -8536,7 +8453,7 @@
         <v>1100.0545909326479</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="A45">
         <v>43</v>
       </c>
@@ -8581,7 +8498,7 @@
         <v>1151.8985665800294</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="A46">
         <v>44</v>
       </c>
@@ -8626,7 +8543,7 @@
         <v>1206.1858735248586</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="A47">
         <v>45</v>
       </c>
@@ -8671,7 +8588,7 @@
         <v>1263.0316624235909</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="A48">
         <v>46</v>
       </c>
@@ -8716,7 +8633,7 @@
         <v>1322.5565108159294</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11">
       <c r="A49">
         <v>47</v>
       </c>
@@ -8761,7 +8678,7 @@
         <v>1384.8866788859477</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11">
       <c r="A50">
         <v>48</v>
       </c>
@@ -8806,7 +8723,7 @@
         <v>1450.1543772768746</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11">
       <c r="A51">
         <v>49</v>
       </c>
@@ -8851,7 +8768,7 @@
         <v>1518.4980475275897</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11">
       <c r="A52">
         <v>50</v>
       </c>
@@ -8896,7 +8813,7 @@
         <v>1590.0626557256919</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11">
       <c r="A53">
         <v>51</v>
       </c>
@@ -8941,7 +8858,7 @@
         <v>1665.0000000000009</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11">
       <c r="A54">
         <v>52</v>
       </c>
@@ -8986,7 +8903,7 @@
         <v>1743.4690325047484</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11">
       <c r="A55">
         <v>53</v>
       </c>
@@ -9031,7 +8948,7 @@
         <v>1825.6361965784051</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11">
       <c r="A56">
         <v>54</v>
       </c>
@@ -9076,7 +8993,7 @@
         <v>1911.6757797923115</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11">
       <c r="A57">
         <v>55</v>
       </c>
@@ -9121,7 +9038,7 @@
         <v>2001.7702836379938</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11">
       <c r="A58">
         <v>56</v>
       </c>
@@ -9166,7 +9083,7 @@
         <v>2096.1108106372894</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11">
       <c r="A59">
         <v>57</v>
       </c>
@@ -9211,7 +9128,7 @@
         <v>2194.8974696964206</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11">
       <c r="A60">
         <v>58</v>
       </c>
@@ -9256,7 +9173,7 @@
         <v>2298.3398005638037</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11">
       <c r="A61">
         <v>59</v>
       </c>
@@ -9301,7 +9218,7 @@
         <v>2406.6572182919713</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11">
       <c r="A62">
         <v>60</v>
       </c>
@@ -9346,7 +9263,7 @@
         <v>2520.0794786462861</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11">
       <c r="A63">
         <v>61</v>
       </c>
@@ -9391,7 +9308,7 @@
         <v>2638.8471654477571</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11">
       <c r="A64">
         <v>62</v>
       </c>
@@ -9436,7 +9353,7 @@
         <v>2763.212200883539</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11">
       <c r="A65">
         <v>63</v>
       </c>
@@ -9481,7 +9398,7 @@
         <v>2893.4383798677127</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11">
       <c r="A66">
         <v>64</v>
       </c>
@@ -9526,7 +9443,7 @@
         <v>3029.8019295856216</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11">
       <c r="A67">
         <v>65</v>
       </c>
@@ -9571,7 +9488,7 @@
         <v>3172.592095408811</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11">
       <c r="A68">
         <v>66</v>
       </c>
@@ -9616,7 +9533,7 @@
         <v>3322.1117544231856</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11">
       <c r="A69">
         <v>67</v>
       </c>
@@ -9661,7 +9578,7 @@
         <v>3478.6780578719795</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11">
       <c r="A70">
         <v>68</v>
       </c>
@@ -9706,7 +9623,7 @@
         <v>3642.6231038760052</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11">
       <c r="A71">
         <v>69</v>
       </c>
@@ -9751,7 +9668,7 @@
         <v>3814.2946418583479</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11">
       <c r="A72">
         <v>70</v>
       </c>
@@ -9796,7 +9713,7 @@
         <v>3994.0568101674535</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11">
       <c r="A73">
         <v>71</v>
       </c>
@@ -9841,7 +9758,7 @@
         <v>4182.2909084634521</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11">
       <c r="A74">
         <v>72</v>
       </c>
@@ -9886,7 +9803,7 @@
         <v>4379.3962065058113</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11">
       <c r="A75">
         <v>73</v>
       </c>
@@ -9931,7 +9848,7 @@
         <v>4585.7907910580507</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11">
       <c r="A76">
         <v>74</v>
       </c>
@@ -9976,7 +9893,7 @@
         <v>4801.9124527058011</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11">
       <c r="A77">
         <v>75</v>
       </c>
@@ -10021,7 +9938,7 @@
         <v>5028.2196144693589</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11">
       <c r="A78">
         <v>76</v>
       </c>
@@ -10066,7 +9983,7 @@
         <v>5265.1923041803529</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11">
       <c r="A79">
         <v>77</v>
       </c>
@@ -10111,7 +10028,7 @@
         <v>5513.333172685142</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11">
       <c r="A80">
         <v>78</v>
       </c>
@@ -10156,7 +10073,7 @@
         <v>5773.1685600346609</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11">
       <c r="A81">
         <v>79</v>
       </c>
@@ -10201,7 +10118,7 @@
         <v>6045.249611922196</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11">
       <c r="A82">
         <v>80</v>
       </c>
@@ -10246,7 +10163,7 @@
         <v>6330.1534487373519</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11">
       <c r="A83">
         <v>81</v>
       </c>
@@ -10291,7 +10208,7 @@
         <v>6628.4843897157361</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11">
       <c r="A84">
         <v>82</v>
       </c>
@@ -10336,7 +10253,7 @@
         <v>6940.8752347810905</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11">
       <c r="A85">
         <v>83</v>
       </c>
@@ -10381,7 +10298,7 @@
         <v>7267.9886067987682</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11">
       <c r="A86">
         <v>84</v>
       </c>
@@ -10426,7 +10343,7 @@
         <v>7610.5183570876734</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11">
       <c r="A87">
         <v>85</v>
       </c>
@@ -10471,7 +10388,7 @@
         <v>7969.1910371719296</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11">
       <c r="A88">
         <v>86</v>
       </c>
@@ -10516,7 +10433,7 @@
         <v>8344.7674398940981</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11">
       <c r="A89">
         <v>87</v>
       </c>
@@ -10561,7 +10478,7 @@
         <v>8738.0442131587133</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11">
       <c r="A90">
         <v>88</v>
       </c>
@@ -10606,7 +10523,7 @@
         <v>9149.8555497294619</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11">
       <c r="A91">
         <v>89</v>
       </c>
@@ -10651,7 +10568,7 @@
         <v>9581.0749566636587</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11">
       <c r="A92">
         <v>90</v>
       </c>
@@ -10696,7 +10613,7 @@
         <v>10032.617108138067</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11">
       <c r="A93">
         <v>91</v>
       </c>
@@ -10741,7 +10658,7 @@
         <v>10505.439785595227</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11">
       <c r="A94">
         <v>92</v>
       </c>
@@ -10786,7 +10703,7 @@
         <v>11000.545909326482</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11">
       <c r="A95">
         <v>93</v>
       </c>
@@ -10831,7 +10748,7 @@
         <v>11518.985665800297</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11">
       <c r="A96">
         <v>94</v>
       </c>
@@ -10876,7 +10793,7 @@
         <v>12061.85873524861</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11">
       <c r="A97">
         <v>95</v>
       </c>
@@ -10921,7 +10838,7 @@
         <v>12630.316624235911</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11">
       <c r="A98">
         <v>96</v>
       </c>
@@ -10966,7 +10883,7 @@
         <v>13225.565108159286</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11">
       <c r="A99">
         <v>97</v>
       </c>
@@ -11011,7 +10928,7 @@
         <v>13848.86678885947</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11">
       <c r="A100">
         <v>98</v>
       </c>
@@ -11056,7 +10973,7 @@
         <v>14501.543772768762</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11">
       <c r="A101">
         <v>99</v>
       </c>
@@ -11101,7 +11018,7 @@
         <v>15184.980475275914</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11">
       <c r="A102">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' into 'Clinton'"
This reverts commit 2db35b4a397699669140ffc9a125ad4e5a644b8d
</commit_message>
<xml_diff>
--- a/misc/LevellingCurves.xlsx
+++ b/misc/LevellingCurves.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louis Thie\workspace\SWEN224\RoomScape\misc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
@@ -10,9 +15,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -76,8 +81,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,11 +131,21 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-NZ"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -159,10 +174,12 @@
         </a:p>
       </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -807,25 +824,35 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:smooth val="0"/>
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-77F1-4892-870A-2398192240AA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:marker val="1"/>
-        <c:axId val="101595008"/>
-        <c:axId val="101596544"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="371007248"/>
+        <c:axId val="371003968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101595008"/>
+        <c:axId val="371007248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -860,17 +887,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101596544"/>
+        <c:crossAx val="371003968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101596544"/>
+        <c:axId val="371003968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -888,6 +917,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -916,7 +946,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101595008"/>
+        <c:crossAx val="371007248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -930,6 +960,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -958,18 +989,28 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-NZ"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -998,10 +1039,12 @@
         </a:p>
       </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1646,25 +1689,35 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:smooth val="0"/>
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3424-4063-ACE7-4E2604062D6B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:marker val="1"/>
-        <c:axId val="101621120"/>
-        <c:axId val="144778368"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="367935632"/>
+        <c:axId val="367927432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101621120"/>
+        <c:axId val="367935632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1699,17 +1752,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="144778368"/>
+        <c:crossAx val="367927432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144778368"/>
+        <c:axId val="367927432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1727,6 +1782,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1755,7 +1811,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101621120"/>
+        <c:crossAx val="367935632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1769,6 +1825,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1797,18 +1854,28 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-NZ"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1837,10 +1904,12 @@
         </a:p>
       </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2485,25 +2554,35 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:smooth val="0"/>
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-922F-4792-A180-AD9CDA08BF87}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:marker val="1"/>
-        <c:axId val="144807040"/>
-        <c:axId val="144808576"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="479235032"/>
+        <c:axId val="479236344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="144807040"/>
+        <c:axId val="479235032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2538,17 +2617,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="144808576"/>
+        <c:crossAx val="479236344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144808576"/>
+        <c:axId val="479236344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2566,6 +2647,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2594,7 +2676,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="144807040"/>
+        <c:crossAx val="479235032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2608,6 +2690,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2636,7 +2719,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4448,7 +4531,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -4500,7 +4583,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -4694,27 +4777,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="15" max="15" width="12.42578125" customWidth="1"/>
     <col min="16" max="16" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4746,7 +4829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4781,7 +4864,7 @@
         <v>1.974</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4798,7 +4881,7 @@
         <v>10.465018489910968</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4815,7 +4898,7 @@
         <v>10.951661199417837</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4832,7 +4915,7 @@
         <v>11.460933694714821</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4849,7 +4932,7 @@
         <v>11.993888302683416</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4866,7 +4949,7 @@
         <v>12.551626285350881</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4883,7 +4966,7 @@
         <v>13.135300115464952</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4900,7 +4983,7 @@
         <v>13.74611585788703</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4917,7 +5000,7 @@
         <v>14.385335661724612</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4934,7 +5017,7 @@
         <v>15.054280368352359</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4951,7 +5034,7 @@
         <v>15.754332240711118</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4968,7 +5051,7 @@
         <v>16.486937819524233</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4985,7 +5068,7 @@
         <v>17.25361091233334</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5002,7 +5085,7 @@
         <v>18.055935721529799</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5019,7 +5102,7 @@
         <v>18.895570117845324</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5036,7 +5119,7 @@
         <v>19.774249066066044</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5053,7 +5136,7 @@
         <v>20.693788210048581</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5070,7 +5153,7 @@
         <v>21.656087624445988</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5087,7 +5170,7 @@
         <v>22.663135740895932</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5104,7 +5187,7 @@
         <v>23.717013456783796</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5121,7 +5204,7 @@
         <v>24.819898435070964</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5138,7 +5221,7 @@
         <v>25.974069604072977</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5155,7 +5238,7 @@
         <v>27.181911866485823</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5172,7 +5255,7 @@
         <v>28.445921027390444</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5189,7 +5272,7 @@
         <v>29.768708951418798</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5206,7 +5289,7 @@
         <v>31.153008959737594</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5223,7 +5306,7 @@
         <v>32.601681478001595</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5240,7 +5323,7 @@
         <v>34.117719946947439</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5257,7 +5340,7 @@
         <v>35.704257007840916</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5274,7 +5357,7 @@
         <v>37.36457097555882</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5291,7 +5374,7 @@
         <v>39.102092612681382</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5308,7 +5391,7 @@
         <v>40.920412218592162</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5325,7 +5408,7 @@
         <v>42.82328704823454</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5342,7 +5425,7 @@
         <v>44.814649075853907</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5359,7 +5442,7 @@
         <v>46.898613119768271</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5376,7 +5459,7 @@
         <v>49.0794853449556</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5393,7 +5476,7 @@
         <v>51.361772161027439</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5410,7 +5493,7 @@
         <v>53.75018953397467</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5427,7 +5510,7 @@
         <v>56.249672730926356</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5444,7 +5527,7 @@
         <v>58.865386518058529</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5461,7 +5544,7 @@
         <v>61.602735832723788</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5478,7 +5561,7 @@
         <v>64.467376951855499</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5495,7 +5578,7 @@
         <v>67.465229179722755</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5512,7 +5595,7 @@
         <v>70.602487079187981</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5529,7 +5612,7 @@
         <v>73.885633271740261</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5546,7 +5629,7 @@
         <v>77.321451832754235</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5563,7 +5646,7 @@
         <v>80.917042309653354</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5580,7 +5663,7 @@
         <v>84.67983439194299</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5597,7 +5680,7 @@
         <v>88.617603263428151</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5614,7 +5697,7 @@
         <v>92.738485668337034</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5631,7 +5714,7 @@
         <v>97.050996724549066</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5648,7 +5731,7 @@
         <v>101.56404751866933</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5665,7 +5748,7 @@
         <v>106.28696351930719</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5682,7 +5765,7 @@
         <v>111.22950384660406</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5699,7 +5782,7 @@
         <v>116.40188143783348</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -5716,7 +5799,7 @@
         <v>121.81478415073521</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5733,7 +5816,7 @@
         <v>127.47939684819566</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5750,7 +5833,7 @@
         <v>133.40742450990646</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5767,7 +5850,7 @@
         <v>139.61111641875721</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5784,7 +5867,7 @@
         <v>146.10329147194074</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5801,7 +5884,7 @@
         <v>152.89736466907115</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5818,7 +5901,7 @@
         <v>160.00737483204873</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -5835,7 +5918,7 @@
         <v>167.44801361395065</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -5852,7 +5935,7 @@
         <v>175.23465585688561</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -5869,7 +5952,7 @@
         <v>183.3833913615492</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -5886,7 +5969,7 @@
         <v>191.9110581341192</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -5903,7 +5986,7 @@
         <v>200.8352771791933</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -5920,7 +6003,7 @@
         <v>210.17448891066547</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -5937,7 +6020,7 @@
         <v>219.94799125577003</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -5954,7 +6037,7 @@
         <v>230.17597953104058</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -5971,7 +6054,7 @@
         <v>240.87958817257109</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -5988,7 +6071,7 @@
         <v>252.08093440680943</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -6005,7 +6088,7 @@
         <v>263.8031639521293</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -6022,7 +6105,7 @@
         <v>276.07049884560485</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -6039,7 +6122,7 @@
         <v>288.90828749381996</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -6056,7 +6139,7 @@
         <v>302.34305705113377</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -6073,7 +6156,7 @@
         <v>316.402568233632</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -6090,7 +6173,7 @@
         <v>331.11587268202788</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -6107,7 +6190,7 @@
         <v>346.51337299204226</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -6124,7 +6207,7 @@
         <v>362.62688553631392</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -6141,7 +6224,7 @@
         <v>379.48970620763509</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -6158,7 +6241,7 @@
         <v>397.13667921937798</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -6175,7 +6258,7 @@
         <v>415.60426910526326</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -6192,7 +6275,7 @@
         <v>434.9306360672511</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -6209,7 +6292,7 @@
         <v>455.15571482725176</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -6226,7 +6309,7 @@
         <v>476.32129714558391</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -6243,7 +6326,7 @@
         <v>498.47111817669042</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -6260,7 +6343,7 @@
         <v>521.65094684056623</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -6277,7 +6360,7 @@
         <v>545.90868039660847</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -6294,7 +6377,7 @@
         <v>571.29444341534065</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -6311,7 +6394,7 @@
         <v>597.86069135249375</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -6328,7 +6411,7 @@
         <v>625.66231893947918</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -6345,7 +6428,7 @@
         <v>654.75677361422299</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -6362,7 +6445,7 @@
         <v>685.20417422672892</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -6379,7 +6462,7 @@
         <v>717.06743526468836</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -6396,7 +6479,7 @@
         <v>750.41239685580081</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -6413,7 +6496,7 @@
         <v>785.30796081543508</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -6430,7 +6513,7 @@
         <v>821.82623302078082</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -6447,7 +6530,7 @@
         <v>860.04267240563524</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -6471,14 +6554,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
@@ -6493,7 +6576,7 @@
     <col min="18" max="18" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -6543,7 +6626,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -6560,10 +6643,10 @@
         <v>45</v>
       </c>
       <c r="R2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -6608,7 +6691,7 @@
         <v>166.49999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -6653,7 +6736,7 @@
         <v>174.34690325047478</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -6698,7 +6781,7 @@
         <v>182.56361965784046</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -6743,7 +6826,7 @@
         <v>191.16757797923108</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -6788,7 +6871,7 @@
         <v>200.17702836379934</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -6833,7 +6916,7 @@
         <v>209.6110810637289</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -6878,7 +6961,7 @@
         <v>219.48974696964197</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -6923,7 +7006,7 @@
         <v>229.83398005638051</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -6968,7 +7051,7 @@
         <v>240.66572182919705</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -7013,7 +7096,7 @@
         <v>252.00794786462879</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -7058,7 +7141,7 @@
         <v>263.8847165447757</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -7103,7 +7186,7 @@
         <v>276.3212200883541</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -7148,7 +7231,7 @@
         <v>289.34383798677118</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -7193,7 +7276,7 @@
         <v>302.98019295856216</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -7238,7 +7321,7 @@
         <v>317.25920954088105</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -7283,7 +7366,7 @@
         <v>332.21117544231851</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -7328,7 +7411,7 @@
         <v>347.86780578719754</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -7373,7 +7456,7 @@
         <v>364.26231038760045</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -7418,7 +7501,7 @@
         <v>381.42946418583438</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -7463,7 +7546,7 @@
         <v>399.40568101674523</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -7508,7 +7591,7 @@
         <v>418.22909084634512</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -7553,7 +7636,7 @@
         <v>437.93962065058099</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -7598,7 +7681,7 @@
         <v>458.57907910580496</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -7643,7 +7726,7 @@
         <v>480.19124527058005</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -7688,7 +7771,7 @@
         <v>502.82196144693575</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -7733,7 +7816,7 @@
         <v>526.51923041803559</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -7778,7 +7861,7 @@
         <v>551.33331726851452</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -7823,7 +7906,7 @@
         <v>577.31685600346543</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -7868,7 +7951,7 @@
         <v>604.52496119221894</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -7913,7 +7996,7 @@
         <v>633.01534487373499</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -7958,7 +8041,7 @@
         <v>662.8484389715735</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -8003,7 +8086,7 @@
         <v>694.08752347810889</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -8048,7 +8131,7 @@
         <v>726.79886067987673</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -8093,7 +8176,7 @@
         <v>761.05183570876784</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -8138,7 +8221,7 @@
         <v>796.91910371719359</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -8183,7 +8266,7 @@
         <v>834.47674398940899</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -8228,7 +8311,7 @@
         <v>873.80442131587108</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -8273,7 +8356,7 @@
         <v>914.98555497294615</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -8318,7 +8401,7 @@
         <v>958.10749566636639</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -8363,7 +8446,7 @@
         <v>1003.2617108138065</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -8408,7 +8491,7 @@
         <v>1050.5439785595215</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -8453,7 +8536,7 @@
         <v>1100.0545909326479</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -8498,7 +8581,7 @@
         <v>1151.8985665800294</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -8543,7 +8626,7 @@
         <v>1206.1858735248586</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -8588,7 +8671,7 @@
         <v>1263.0316624235909</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -8633,7 +8716,7 @@
         <v>1322.5565108159294</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -8678,7 +8761,7 @@
         <v>1384.8866788859477</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -8723,7 +8806,7 @@
         <v>1450.1543772768746</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -8768,7 +8851,7 @@
         <v>1518.4980475275897</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -8813,7 +8896,7 @@
         <v>1590.0626557256919</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -8858,7 +8941,7 @@
         <v>1665.0000000000009</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -8903,7 +8986,7 @@
         <v>1743.4690325047484</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -8948,7 +9031,7 @@
         <v>1825.6361965784051</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -8993,7 +9076,7 @@
         <v>1911.6757797923115</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -9038,7 +9121,7 @@
         <v>2001.7702836379938</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -9083,7 +9166,7 @@
         <v>2096.1108106372894</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -9128,7 +9211,7 @@
         <v>2194.8974696964206</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -9173,7 +9256,7 @@
         <v>2298.3398005638037</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -9218,7 +9301,7 @@
         <v>2406.6572182919713</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -9263,7 +9346,7 @@
         <v>2520.0794786462861</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -9308,7 +9391,7 @@
         <v>2638.8471654477571</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -9353,7 +9436,7 @@
         <v>2763.212200883539</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -9398,7 +9481,7 @@
         <v>2893.4383798677127</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -9443,7 +9526,7 @@
         <v>3029.8019295856216</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -9488,7 +9571,7 @@
         <v>3172.592095408811</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -9533,7 +9616,7 @@
         <v>3322.1117544231856</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -9578,7 +9661,7 @@
         <v>3478.6780578719795</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -9623,7 +9706,7 @@
         <v>3642.6231038760052</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -9668,7 +9751,7 @@
         <v>3814.2946418583479</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -9713,7 +9796,7 @@
         <v>3994.0568101674535</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -9758,7 +9841,7 @@
         <v>4182.2909084634521</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -9803,7 +9886,7 @@
         <v>4379.3962065058113</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -9848,7 +9931,7 @@
         <v>4585.7907910580507</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -9893,7 +9976,7 @@
         <v>4801.9124527058011</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -9938,7 +10021,7 @@
         <v>5028.2196144693589</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -9983,7 +10066,7 @@
         <v>5265.1923041803529</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -10028,7 +10111,7 @@
         <v>5513.333172685142</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -10073,7 +10156,7 @@
         <v>5773.1685600346609</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -10118,7 +10201,7 @@
         <v>6045.249611922196</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -10163,7 +10246,7 @@
         <v>6330.1534487373519</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -10208,7 +10291,7 @@
         <v>6628.4843897157361</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -10253,7 +10336,7 @@
         <v>6940.8752347810905</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -10298,7 +10381,7 @@
         <v>7267.9886067987682</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -10343,7 +10426,7 @@
         <v>7610.5183570876734</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -10388,7 +10471,7 @@
         <v>7969.1910371719296</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -10433,7 +10516,7 @@
         <v>8344.7674398940981</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -10478,7 +10561,7 @@
         <v>8738.0442131587133</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -10523,7 +10606,7 @@
         <v>9149.8555497294619</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -10568,7 +10651,7 @@
         <v>9581.0749566636587</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
@@ -10613,7 +10696,7 @@
         <v>10032.617108138067</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -10658,7 +10741,7 @@
         <v>10505.439785595227</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -10703,7 +10786,7 @@
         <v>11000.545909326482</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -10748,7 +10831,7 @@
         <v>11518.985665800297</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -10793,7 +10876,7 @@
         <v>12061.85873524861</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -10838,7 +10921,7 @@
         <v>12630.316624235911</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -10883,7 +10966,7 @@
         <v>13225.565108159286</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -10928,7 +11011,7 @@
         <v>13848.86678885947</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -10973,7 +11056,7 @@
         <v>14501.543772768762</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -11018,7 +11101,7 @@
         <v>15184.980475275914</v>
       </c>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Revert "Merge branch 'Clinton' into 'master'"
This reverts merge request !77
</commit_message>
<xml_diff>
--- a/misc/LevellingCurves.xlsx
+++ b/misc/LevellingCurves.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louis Thie\workspace\SWEN224\RoomScape\misc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
@@ -15,9 +10,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -81,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,21 +126,11 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-NZ"/>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -174,12 +159,10 @@
         </a:p>
       </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -824,35 +807,25 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-77F1-4892-870A-2398192240AA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="371007248"/>
-        <c:axId val="371003968"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="101595008"/>
+        <c:axId val="101596544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="371007248"/>
+        <c:axId val="101595008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -887,19 +860,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371003968"/>
+        <c:crossAx val="101596544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="371003968"/>
+        <c:axId val="101596544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -917,7 +888,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -946,7 +916,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371007248"/>
+        <c:crossAx val="101595008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -960,7 +930,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -989,28 +958,18 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-NZ"/>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1039,12 +998,10 @@
         </a:p>
       </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1689,35 +1646,25 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3424-4063-ACE7-4E2604062D6B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="367935632"/>
-        <c:axId val="367927432"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="101621120"/>
+        <c:axId val="144778368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="367935632"/>
+        <c:axId val="101621120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1752,19 +1699,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="367927432"/>
+        <c:crossAx val="144778368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="367927432"/>
+        <c:axId val="144778368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1782,7 +1727,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1811,7 +1755,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="367935632"/>
+        <c:crossAx val="101621120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1825,7 +1769,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1854,28 +1797,18 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-NZ"/>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1904,12 +1837,10 @@
         </a:p>
       </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2554,35 +2485,25 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-922F-4792-A180-AD9CDA08BF87}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="479235032"/>
-        <c:axId val="479236344"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="144807040"/>
+        <c:axId val="144808576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="479235032"/>
+        <c:axId val="144807040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2617,19 +2538,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479236344"/>
+        <c:crossAx val="144808576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="479236344"/>
+        <c:axId val="144808576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2647,7 +2566,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2676,7 +2594,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479235032"/>
+        <c:crossAx val="144807040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2690,7 +2608,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2719,7 +2636,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4531,7 +4448,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -4583,7 +4500,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -4777,27 +4694,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="15" max="15" width="12.42578125" customWidth="1"/>
     <col min="16" max="16" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4829,7 +4746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4864,7 +4781,7 @@
         <v>1.974</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4881,7 +4798,7 @@
         <v>10.465018489910968</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4898,7 +4815,7 @@
         <v>10.951661199417837</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4915,7 +4832,7 @@
         <v>11.460933694714821</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4932,7 +4849,7 @@
         <v>11.993888302683416</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4949,7 +4866,7 @@
         <v>12.551626285350881</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4966,7 +4883,7 @@
         <v>13.135300115464952</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4983,7 +4900,7 @@
         <v>13.74611585788703</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5000,7 +4917,7 @@
         <v>14.385335661724612</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5017,7 +4934,7 @@
         <v>15.054280368352359</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5034,7 +4951,7 @@
         <v>15.754332240711118</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5051,7 +4968,7 @@
         <v>16.486937819524233</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5068,7 +4985,7 @@
         <v>17.25361091233334</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5085,7 +5002,7 @@
         <v>18.055935721529799</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5102,7 +5019,7 @@
         <v>18.895570117845324</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5119,7 +5036,7 @@
         <v>19.774249066066044</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5136,7 +5053,7 @@
         <v>20.693788210048581</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5153,7 +5070,7 @@
         <v>21.656087624445988</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5170,7 +5087,7 @@
         <v>22.663135740895932</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5187,7 +5104,7 @@
         <v>23.717013456783796</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5204,7 +5121,7 @@
         <v>24.819898435070964</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5221,7 +5138,7 @@
         <v>25.974069604072977</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5238,7 +5155,7 @@
         <v>27.181911866485823</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5255,7 +5172,7 @@
         <v>28.445921027390444</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5272,7 +5189,7 @@
         <v>29.768708951418798</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5289,7 +5206,7 @@
         <v>31.153008959737594</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5306,7 +5223,7 @@
         <v>32.601681478001595</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5323,7 +5240,7 @@
         <v>34.117719946947439</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5340,7 +5257,7 @@
         <v>35.704257007840916</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5357,7 +5274,7 @@
         <v>37.36457097555882</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5374,7 +5291,7 @@
         <v>39.102092612681382</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5391,7 +5308,7 @@
         <v>40.920412218592162</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5408,7 +5325,7 @@
         <v>42.82328704823454</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5425,7 +5342,7 @@
         <v>44.814649075853907</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5442,7 +5359,7 @@
         <v>46.898613119768271</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5459,7 +5376,7 @@
         <v>49.0794853449556</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5476,7 +5393,7 @@
         <v>51.361772161027439</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5493,7 +5410,7 @@
         <v>53.75018953397467</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5510,7 +5427,7 @@
         <v>56.249672730926356</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5527,7 +5444,7 @@
         <v>58.865386518058529</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5544,7 +5461,7 @@
         <v>61.602735832723788</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5561,7 +5478,7 @@
         <v>64.467376951855499</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5578,7 +5495,7 @@
         <v>67.465229179722755</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5595,7 +5512,7 @@
         <v>70.602487079187981</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5612,7 +5529,7 @@
         <v>73.885633271740261</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5629,7 +5546,7 @@
         <v>77.321451832754235</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5646,7 +5563,7 @@
         <v>80.917042309653354</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5663,7 +5580,7 @@
         <v>84.67983439194299</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5680,7 +5597,7 @@
         <v>88.617603263428151</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5697,7 +5614,7 @@
         <v>92.738485668337034</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5714,7 +5631,7 @@
         <v>97.050996724549066</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5731,7 +5648,7 @@
         <v>101.56404751866933</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5748,7 +5665,7 @@
         <v>106.28696351930719</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5765,7 +5682,7 @@
         <v>111.22950384660406</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5782,7 +5699,7 @@
         <v>116.40188143783348</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>56</v>
       </c>
@@ -5799,7 +5716,7 @@
         <v>121.81478415073521</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5816,7 +5733,7 @@
         <v>127.47939684819566</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5833,7 +5750,7 @@
         <v>133.40742450990646</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5850,7 +5767,7 @@
         <v>139.61111641875721</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5867,7 +5784,7 @@
         <v>146.10329147194074</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5884,7 +5801,7 @@
         <v>152.89736466907115</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5901,7 +5818,7 @@
         <v>160.00737483204873</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64">
         <v>63</v>
       </c>
@@ -5918,7 +5835,7 @@
         <v>167.44801361395065</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65">
         <v>64</v>
       </c>
@@ -5935,7 +5852,7 @@
         <v>175.23465585688561</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66">
         <v>65</v>
       </c>
@@ -5952,7 +5869,7 @@
         <v>183.3833913615492</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67">
         <v>66</v>
       </c>
@@ -5969,7 +5886,7 @@
         <v>191.9110581341192</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68">
         <v>67</v>
       </c>
@@ -5986,7 +5903,7 @@
         <v>200.8352771791933</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69">
         <v>68</v>
       </c>
@@ -6003,7 +5920,7 @@
         <v>210.17448891066547</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70">
         <v>69</v>
       </c>
@@ -6020,7 +5937,7 @@
         <v>219.94799125577003</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71">
         <v>70</v>
       </c>
@@ -6037,7 +5954,7 @@
         <v>230.17597953104058</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6054,7 +5971,7 @@
         <v>240.87958817257109</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6071,7 +5988,7 @@
         <v>252.08093440680943</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74">
         <v>73</v>
       </c>
@@ -6088,7 +6005,7 @@
         <v>263.8031639521293</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75">
         <v>74</v>
       </c>
@@ -6105,7 +6022,7 @@
         <v>276.07049884560485</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76">
         <v>75</v>
       </c>
@@ -6122,7 +6039,7 @@
         <v>288.90828749381996</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77">
         <v>76</v>
       </c>
@@ -6139,7 +6056,7 @@
         <v>302.34305705113377</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78">
         <v>77</v>
       </c>
@@ -6156,7 +6073,7 @@
         <v>316.402568233632</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79">
         <v>78</v>
       </c>
@@ -6173,7 +6090,7 @@
         <v>331.11587268202788</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80">
         <v>79</v>
       </c>
@@ -6190,7 +6107,7 @@
         <v>346.51337299204226</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81">
         <v>80</v>
       </c>
@@ -6207,7 +6124,7 @@
         <v>362.62688553631392</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82">
         <v>81</v>
       </c>
@@ -6224,7 +6141,7 @@
         <v>379.48970620763509</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4">
       <c r="A83">
         <v>82</v>
       </c>
@@ -6241,7 +6158,7 @@
         <v>397.13667921937798</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84">
         <v>83</v>
       </c>
@@ -6258,7 +6175,7 @@
         <v>415.60426910526326</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85">
         <v>84</v>
       </c>
@@ -6275,7 +6192,7 @@
         <v>434.9306360672511</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86">
         <v>85</v>
       </c>
@@ -6292,7 +6209,7 @@
         <v>455.15571482725176</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87">
         <v>86</v>
       </c>
@@ -6309,7 +6226,7 @@
         <v>476.32129714558391</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88">
         <v>87</v>
       </c>
@@ -6326,7 +6243,7 @@
         <v>498.47111817669042</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89">
         <v>88</v>
       </c>
@@ -6343,7 +6260,7 @@
         <v>521.65094684056623</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90">
         <v>89</v>
       </c>
@@ -6360,7 +6277,7 @@
         <v>545.90868039660847</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91">
         <v>90</v>
       </c>
@@ -6377,7 +6294,7 @@
         <v>571.29444341534065</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92">
         <v>91</v>
       </c>
@@ -6394,7 +6311,7 @@
         <v>597.86069135249375</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93">
         <v>92</v>
       </c>
@@ -6411,7 +6328,7 @@
         <v>625.66231893947918</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94">
         <v>93</v>
       </c>
@@ -6428,7 +6345,7 @@
         <v>654.75677361422299</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95">
         <v>94</v>
       </c>
@@ -6445,7 +6362,7 @@
         <v>685.20417422672892</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96">
         <v>95</v>
       </c>
@@ -6462,7 +6379,7 @@
         <v>717.06743526468836</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97">
         <v>96</v>
       </c>
@@ -6479,7 +6396,7 @@
         <v>750.41239685580081</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98">
         <v>97</v>
       </c>
@@ -6496,7 +6413,7 @@
         <v>785.30796081543508</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99">
         <v>98</v>
       </c>
@@ -6513,7 +6430,7 @@
         <v>821.82623302078082</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100">
         <v>99</v>
       </c>
@@ -6530,7 +6447,7 @@
         <v>860.04267240563524</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101">
         <v>100</v>
       </c>
@@ -6554,14 +6471,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
@@ -6576,7 +6493,7 @@
     <col min="18" max="18" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -6626,7 +6543,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -6643,10 +6560,10 @@
         <v>45</v>
       </c>
       <c r="R2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>1</v>
       </c>
@@ -6691,7 +6608,7 @@
         <v>166.49999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>2</v>
       </c>
@@ -6736,7 +6653,7 @@
         <v>174.34690325047478</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>3</v>
       </c>
@@ -6781,7 +6698,7 @@
         <v>182.56361965784046</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>4</v>
       </c>
@@ -6826,7 +6743,7 @@
         <v>191.16757797923108</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>5</v>
       </c>
@@ -6871,7 +6788,7 @@
         <v>200.17702836379934</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>6</v>
       </c>
@@ -6916,7 +6833,7 @@
         <v>209.6110810637289</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>7</v>
       </c>
@@ -6961,7 +6878,7 @@
         <v>219.48974696964197</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>8</v>
       </c>
@@ -7006,7 +6923,7 @@
         <v>229.83398005638051</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>9</v>
       </c>
@@ -7051,7 +6968,7 @@
         <v>240.66572182919705</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>10</v>
       </c>
@@ -7096,7 +7013,7 @@
         <v>252.00794786462879</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>11</v>
       </c>
@@ -7141,7 +7058,7 @@
         <v>263.8847165447757</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>12</v>
       </c>
@@ -7186,7 +7103,7 @@
         <v>276.3212200883541</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>13</v>
       </c>
@@ -7231,7 +7148,7 @@
         <v>289.34383798677118</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>14</v>
       </c>
@@ -7276,7 +7193,7 @@
         <v>302.98019295856216</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>15</v>
       </c>
@@ -7321,7 +7238,7 @@
         <v>317.25920954088105</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>16</v>
       </c>
@@ -7366,7 +7283,7 @@
         <v>332.21117544231851</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>17</v>
       </c>
@@ -7411,7 +7328,7 @@
         <v>347.86780578719754</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>18</v>
       </c>
@@ -7456,7 +7373,7 @@
         <v>364.26231038760045</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>19</v>
       </c>
@@ -7501,7 +7418,7 @@
         <v>381.42946418583438</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>20</v>
       </c>
@@ -7546,7 +7463,7 @@
         <v>399.40568101674523</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>21</v>
       </c>
@@ -7591,7 +7508,7 @@
         <v>418.22909084634512</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>22</v>
       </c>
@@ -7636,7 +7553,7 @@
         <v>437.93962065058099</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>23</v>
       </c>
@@ -7681,7 +7598,7 @@
         <v>458.57907910580496</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>24</v>
       </c>
@@ -7726,7 +7643,7 @@
         <v>480.19124527058005</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>25</v>
       </c>
@@ -7771,7 +7688,7 @@
         <v>502.82196144693575</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>26</v>
       </c>
@@ -7816,7 +7733,7 @@
         <v>526.51923041803559</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>27</v>
       </c>
@@ -7861,7 +7778,7 @@
         <v>551.33331726851452</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>28</v>
       </c>
@@ -7906,7 +7823,7 @@
         <v>577.31685600346543</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31">
         <v>29</v>
       </c>
@@ -7951,7 +7868,7 @@
         <v>604.52496119221894</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32">
         <v>30</v>
       </c>
@@ -7996,7 +7913,7 @@
         <v>633.01534487373499</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33">
         <v>31</v>
       </c>
@@ -8041,7 +7958,7 @@
         <v>662.8484389715735</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34">
         <v>32</v>
       </c>
@@ -8086,7 +8003,7 @@
         <v>694.08752347810889</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35">
         <v>33</v>
       </c>
@@ -8131,7 +8048,7 @@
         <v>726.79886067987673</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36">
         <v>34</v>
       </c>
@@ -8176,7 +8093,7 @@
         <v>761.05183570876784</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37">
         <v>35</v>
       </c>
@@ -8221,7 +8138,7 @@
         <v>796.91910371719359</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38">
         <v>36</v>
       </c>
@@ -8266,7 +8183,7 @@
         <v>834.47674398940899</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39">
         <v>37</v>
       </c>
@@ -8311,7 +8228,7 @@
         <v>873.80442131587108</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40">
         <v>38</v>
       </c>
@@ -8356,7 +8273,7 @@
         <v>914.98555497294615</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41">
         <v>39</v>
       </c>
@@ -8401,7 +8318,7 @@
         <v>958.10749566636639</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42">
         <v>40</v>
       </c>
@@ -8446,7 +8363,7 @@
         <v>1003.2617108138065</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43">
         <v>41</v>
       </c>
@@ -8491,7 +8408,7 @@
         <v>1050.5439785595215</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="A44">
         <v>42</v>
       </c>
@@ -8536,7 +8453,7 @@
         <v>1100.0545909326479</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="A45">
         <v>43</v>
       </c>
@@ -8581,7 +8498,7 @@
         <v>1151.8985665800294</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="A46">
         <v>44</v>
       </c>
@@ -8626,7 +8543,7 @@
         <v>1206.1858735248586</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="A47">
         <v>45</v>
       </c>
@@ -8671,7 +8588,7 @@
         <v>1263.0316624235909</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="A48">
         <v>46</v>
       </c>
@@ -8716,7 +8633,7 @@
         <v>1322.5565108159294</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11">
       <c r="A49">
         <v>47</v>
       </c>
@@ -8761,7 +8678,7 @@
         <v>1384.8866788859477</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11">
       <c r="A50">
         <v>48</v>
       </c>
@@ -8806,7 +8723,7 @@
         <v>1450.1543772768746</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11">
       <c r="A51">
         <v>49</v>
       </c>
@@ -8851,7 +8768,7 @@
         <v>1518.4980475275897</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11">
       <c r="A52">
         <v>50</v>
       </c>
@@ -8896,7 +8813,7 @@
         <v>1590.0626557256919</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11">
       <c r="A53">
         <v>51</v>
       </c>
@@ -8941,7 +8858,7 @@
         <v>1665.0000000000009</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11">
       <c r="A54">
         <v>52</v>
       </c>
@@ -8986,7 +8903,7 @@
         <v>1743.4690325047484</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11">
       <c r="A55">
         <v>53</v>
       </c>
@@ -9031,7 +8948,7 @@
         <v>1825.6361965784051</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11">
       <c r="A56">
         <v>54</v>
       </c>
@@ -9076,7 +8993,7 @@
         <v>1911.6757797923115</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11">
       <c r="A57">
         <v>55</v>
       </c>
@@ -9121,7 +9038,7 @@
         <v>2001.7702836379938</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11">
       <c r="A58">
         <v>56</v>
       </c>
@@ -9166,7 +9083,7 @@
         <v>2096.1108106372894</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11">
       <c r="A59">
         <v>57</v>
       </c>
@@ -9211,7 +9128,7 @@
         <v>2194.8974696964206</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11">
       <c r="A60">
         <v>58</v>
       </c>
@@ -9256,7 +9173,7 @@
         <v>2298.3398005638037</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11">
       <c r="A61">
         <v>59</v>
       </c>
@@ -9301,7 +9218,7 @@
         <v>2406.6572182919713</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11">
       <c r="A62">
         <v>60</v>
       </c>
@@ -9346,7 +9263,7 @@
         <v>2520.0794786462861</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11">
       <c r="A63">
         <v>61</v>
       </c>
@@ -9391,7 +9308,7 @@
         <v>2638.8471654477571</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11">
       <c r="A64">
         <v>62</v>
       </c>
@@ -9436,7 +9353,7 @@
         <v>2763.212200883539</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11">
       <c r="A65">
         <v>63</v>
       </c>
@@ -9481,7 +9398,7 @@
         <v>2893.4383798677127</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11">
       <c r="A66">
         <v>64</v>
       </c>
@@ -9526,7 +9443,7 @@
         <v>3029.8019295856216</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11">
       <c r="A67">
         <v>65</v>
       </c>
@@ -9571,7 +9488,7 @@
         <v>3172.592095408811</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11">
       <c r="A68">
         <v>66</v>
       </c>
@@ -9616,7 +9533,7 @@
         <v>3322.1117544231856</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11">
       <c r="A69">
         <v>67</v>
       </c>
@@ -9661,7 +9578,7 @@
         <v>3478.6780578719795</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11">
       <c r="A70">
         <v>68</v>
       </c>
@@ -9706,7 +9623,7 @@
         <v>3642.6231038760052</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11">
       <c r="A71">
         <v>69</v>
       </c>
@@ -9751,7 +9668,7 @@
         <v>3814.2946418583479</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11">
       <c r="A72">
         <v>70</v>
       </c>
@@ -9796,7 +9713,7 @@
         <v>3994.0568101674535</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11">
       <c r="A73">
         <v>71</v>
       </c>
@@ -9841,7 +9758,7 @@
         <v>4182.2909084634521</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11">
       <c r="A74">
         <v>72</v>
       </c>
@@ -9886,7 +9803,7 @@
         <v>4379.3962065058113</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11">
       <c r="A75">
         <v>73</v>
       </c>
@@ -9931,7 +9848,7 @@
         <v>4585.7907910580507</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11">
       <c r="A76">
         <v>74</v>
       </c>
@@ -9976,7 +9893,7 @@
         <v>4801.9124527058011</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11">
       <c r="A77">
         <v>75</v>
       </c>
@@ -10021,7 +9938,7 @@
         <v>5028.2196144693589</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11">
       <c r="A78">
         <v>76</v>
       </c>
@@ -10066,7 +9983,7 @@
         <v>5265.1923041803529</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11">
       <c r="A79">
         <v>77</v>
       </c>
@@ -10111,7 +10028,7 @@
         <v>5513.333172685142</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11">
       <c r="A80">
         <v>78</v>
       </c>
@@ -10156,7 +10073,7 @@
         <v>5773.1685600346609</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11">
       <c r="A81">
         <v>79</v>
       </c>
@@ -10201,7 +10118,7 @@
         <v>6045.249611922196</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11">
       <c r="A82">
         <v>80</v>
       </c>
@@ -10246,7 +10163,7 @@
         <v>6330.1534487373519</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11">
       <c r="A83">
         <v>81</v>
       </c>
@@ -10291,7 +10208,7 @@
         <v>6628.4843897157361</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11">
       <c r="A84">
         <v>82</v>
       </c>
@@ -10336,7 +10253,7 @@
         <v>6940.8752347810905</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11">
       <c r="A85">
         <v>83</v>
       </c>
@@ -10381,7 +10298,7 @@
         <v>7267.9886067987682</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11">
       <c r="A86">
         <v>84</v>
       </c>
@@ -10426,7 +10343,7 @@
         <v>7610.5183570876734</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11">
       <c r="A87">
         <v>85</v>
       </c>
@@ -10471,7 +10388,7 @@
         <v>7969.1910371719296</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11">
       <c r="A88">
         <v>86</v>
       </c>
@@ -10516,7 +10433,7 @@
         <v>8344.7674398940981</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11">
       <c r="A89">
         <v>87</v>
       </c>
@@ -10561,7 +10478,7 @@
         <v>8738.0442131587133</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11">
       <c r="A90">
         <v>88</v>
       </c>
@@ -10606,7 +10523,7 @@
         <v>9149.8555497294619</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11">
       <c r="A91">
         <v>89</v>
       </c>
@@ -10651,7 +10568,7 @@
         <v>9581.0749566636587</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11">
       <c r="A92">
         <v>90</v>
       </c>
@@ -10696,7 +10613,7 @@
         <v>10032.617108138067</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11">
       <c r="A93">
         <v>91</v>
       </c>
@@ -10741,7 +10658,7 @@
         <v>10505.439785595227</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11">
       <c r="A94">
         <v>92</v>
       </c>
@@ -10786,7 +10703,7 @@
         <v>11000.545909326482</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11">
       <c r="A95">
         <v>93</v>
       </c>
@@ -10831,7 +10748,7 @@
         <v>11518.985665800297</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11">
       <c r="A96">
         <v>94</v>
       </c>
@@ -10876,7 +10793,7 @@
         <v>12061.85873524861</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11">
       <c r="A97">
         <v>95</v>
       </c>
@@ -10921,7 +10838,7 @@
         <v>12630.316624235911</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11">
       <c r="A98">
         <v>96</v>
       </c>
@@ -10966,7 +10883,7 @@
         <v>13225.565108159286</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11">
       <c r="A99">
         <v>97</v>
       </c>
@@ -11011,7 +10928,7 @@
         <v>13848.86678885947</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11">
       <c r="A100">
         <v>98</v>
       </c>
@@ -11056,7 +10973,7 @@
         <v>14501.543772768762</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11">
       <c r="A101">
         <v>99</v>
       </c>
@@ -11101,7 +11018,7 @@
         <v>15184.980475275914</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11">
       <c r="A102">
         <v>100</v>
       </c>

</xml_diff>